<commit_message>
add main.py for run once.
</commit_message>
<xml_diff>
--- a/Fund.xlsx
+++ b/Fund.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12465" windowWidth="27975"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8235" windowWidth="19185"/>
   </bookViews>
   <sheets>
     <sheet name="基金" sheetId="1" state="visible" r:id="rId1"/>
@@ -80,8 +80,83 @@
     <font>
       <name val="宋体"/>
       <charset val="134"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
       <b val="1"/>
       <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -95,37 +170,8 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
       <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -139,24 +185,16 @@
     </font>
     <font>
       <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="0"/>
       <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -176,48 +214,14 @@
     </font>
     <font>
       <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <color rgb="00FF0000"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill/>
     </fill>
@@ -268,37 +272,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,19 +404,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,115 +422,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,23 +475,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -490,7 +485,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,6 +501,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -527,9 +531,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,171 +569,161 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="38" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="34" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="9" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="9" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="31" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="36" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="35" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="21" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="28" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="40" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="44">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="33" fontId="12" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="26" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="23" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="39" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="36" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="18" fontId="22" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="31" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="20" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="37" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="23" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="24" fontId="21" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="37" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="34" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="24" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="18" fontId="22" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="22" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="33" fontId="23" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="19" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="21" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="27" fontId="19" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="5" fillId="18" fontId="16" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="15" numFmtId="0">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="25" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="42">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="43">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="20" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="24" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="43">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="14" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="13" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="38" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="12" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="41">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="39" fontId="9" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="10" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="10" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="11" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="41">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="7" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="35" fontId="9" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="20" numFmtId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -737,7 +748,6 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="3" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -786,19 +796,22 @@
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="3" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="31">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="7" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="4" numFmtId="10" pivotButton="0" quotePrefix="0" xfId="0">
@@ -870,9 +883,6 @@
     <xf applyAlignment="1" borderId="0" fillId="8" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -893,9 +903,6 @@
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="168" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="25" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="4" numFmtId="166" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -1267,26 +1274,26 @@
   </sheetPr>
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="9" width="8.875"/>
-    <col customWidth="1" max="2" min="2" style="9" width="28.5"/>
-    <col customWidth="1" max="5" min="5" style="9" width="9.875"/>
-    <col customWidth="1" max="6" min="6" style="9" width="9.375"/>
-    <col customWidth="1" max="7" min="7" style="9" width="10.375"/>
-    <col customWidth="1" max="10" min="8" style="9" width="9.875"/>
-    <col customWidth="1" max="11" min="11" style="9" width="16"/>
-    <col customWidth="1" max="13" min="12" style="9" width="9.375"/>
-    <col customWidth="1" max="14" min="14" style="9" width="11.25"/>
-    <col customWidth="1" max="15" min="15" style="9" width="15.625"/>
-    <col customWidth="1" max="17" min="17" style="9" width="19.125"/>
-    <col customWidth="1" max="18" min="18" style="9" width="9.375"/>
-    <col customWidth="1" max="19" min="19" style="9" width="19.125"/>
-    <col customWidth="1" max="20" min="20" style="9" width="12"/>
+    <col customWidth="1" max="1" min="1" style="1" width="8.875"/>
+    <col customWidth="1" max="2" min="2" style="1" width="28.5"/>
+    <col customWidth="1" max="5" min="5" style="1" width="9.875"/>
+    <col customWidth="1" max="6" min="6" style="1" width="9.375"/>
+    <col customWidth="1" max="7" min="7" style="1" width="10.375"/>
+    <col customWidth="1" max="10" min="8" style="1" width="9.875"/>
+    <col customWidth="1" max="11" min="11" style="1" width="16"/>
+    <col customWidth="1" max="13" min="12" style="1" width="9.375"/>
+    <col customWidth="1" max="14" min="14" style="1" width="11.25"/>
+    <col customWidth="1" max="15" min="15" style="1" width="15.625"/>
+    <col customWidth="1" max="17" min="17" style="1" width="19.125"/>
+    <col customWidth="1" max="18" min="18" style="1" width="9.375"/>
+    <col customWidth="1" max="19" min="19" style="1" width="19.125"/>
+    <col customWidth="1" max="20" min="20" style="1" width="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1305,52 +1312,52 @@
           <t>类型</t>
         </is>
       </c>
-      <c r="D1" s="45" t="inlineStr">
+      <c r="D1" s="46" t="inlineStr">
         <is>
           <t>1年夏普</t>
         </is>
       </c>
-      <c r="E1" s="45" t="inlineStr">
+      <c r="E1" s="46" t="inlineStr">
         <is>
           <t>成本单价</t>
         </is>
       </c>
-      <c r="F1" s="45" t="inlineStr">
+      <c r="F1" s="46" t="inlineStr">
         <is>
           <t>份额</t>
         </is>
       </c>
-      <c r="G1" s="45" t="inlineStr">
+      <c r="G1" s="46" t="inlineStr">
         <is>
           <t>成本</t>
         </is>
       </c>
-      <c r="H1" s="45" t="inlineStr">
+      <c r="H1" s="46" t="inlineStr">
         <is>
           <t>最新净值</t>
         </is>
       </c>
-      <c r="I1" s="46" t="inlineStr">
+      <c r="I1" s="47" t="inlineStr">
         <is>
           <t>估值</t>
         </is>
       </c>
-      <c r="J1" s="46" t="inlineStr">
+      <c r="J1" s="47" t="inlineStr">
         <is>
           <t>较昨日涨跌</t>
         </is>
       </c>
-      <c r="K1" s="46" t="inlineStr">
+      <c r="K1" s="47" t="inlineStr">
         <is>
           <t>成本单价涨跌</t>
         </is>
       </c>
-      <c r="L1" s="45" t="inlineStr">
+      <c r="L1" s="46" t="inlineStr">
         <is>
           <t>资产</t>
         </is>
       </c>
-      <c r="M1" s="45" t="inlineStr">
+      <c r="M1" s="46" t="inlineStr">
         <is>
           <t>收益</t>
         </is>
@@ -1370,7 +1377,7 @@
           <t>持有天数</t>
         </is>
       </c>
-      <c r="Q1" s="45" t="inlineStr">
+      <c r="Q1" s="46" t="inlineStr">
         <is>
           <t>操作策略</t>
         </is>
@@ -1388,7 +1395,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="8" t="inlineStr">
+      <c r="A2" s="9" t="inlineStr">
         <is>
           <t>161903</t>
         </is>
@@ -1403,52 +1410,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D2" s="47" t="n">
+      <c r="D2" s="48" t="n">
         <v>0.45</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1.2457</v>
       </c>
-      <c r="F2" s="48" t="n">
+      <c r="F2" s="49" t="n">
         <v>6391.45</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G2" s="49">
         <f>E2*F2</f>
         <v/>
       </c>
       <c r="H2" s="0" t="n">
-        <v>1.6297</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>1.6413</v>
-      </c>
-      <c r="J2" s="26" t="n">
-        <v>0.0071</v>
+        <v>1.6048</v>
+      </c>
+      <c r="I2" s="26" t="n">
+        <v>1.6012</v>
+      </c>
+      <c r="J2" s="27" t="n">
+        <v>-0.0023</v>
       </c>
       <c r="K2" s="27">
         <f>(I2-E2)/E2</f>
         <v/>
       </c>
-      <c r="L2" s="48">
+      <c r="L2" s="49">
         <f>H2*F2</f>
         <v/>
       </c>
-      <c r="M2" s="48">
+      <c r="M2" s="49">
         <f>L2-G2</f>
         <v/>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="29">
         <f>M2/G2</f>
         <v/>
       </c>
-      <c r="O2" s="49" t="n">
+      <c r="O2" s="50" t="n">
         <v>43822</v>
       </c>
-      <c r="P2" s="50">
+      <c r="P2" s="51">
         <f>TODAY()-O2</f>
         <v/>
       </c>
-      <c r="Q2" s="48" t="inlineStr">
+      <c r="Q2" s="49" t="inlineStr">
         <is>
           <t>择时加仓</t>
         </is>
@@ -1458,7 +1465,7 @@
       <c r="T2" s="0" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="8" t="n">
+      <c r="A3" s="9" t="n">
         <v>161706</v>
       </c>
       <c r="B3" s="15" t="inlineStr">
@@ -1471,52 +1478,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D3" s="51" t="n">
+      <c r="D3" s="52" t="n">
         <v>0.36</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1.6753</v>
       </c>
-      <c r="F3" s="48" t="n">
+      <c r="F3" s="49" t="n">
         <v>5109.2</v>
       </c>
-      <c r="G3" s="48">
+      <c r="G3" s="49">
         <f>E3*F3</f>
         <v/>
       </c>
       <c r="H3" s="0" t="n">
-        <v>1.9527</v>
-      </c>
-      <c r="I3" s="0" t="n">
-        <v>1.9671</v>
-      </c>
-      <c r="J3" s="26" t="n">
-        <v>0.0074</v>
+        <v>1.9394</v>
+      </c>
+      <c r="I3" s="26" t="n">
+        <v>1.9257</v>
+      </c>
+      <c r="J3" s="27" t="n">
+        <v>-0.0071</v>
       </c>
       <c r="K3" s="27">
         <f>(I3-E3)/E3</f>
         <v/>
       </c>
-      <c r="L3" s="48">
+      <c r="L3" s="49">
         <f>H3*F3</f>
         <v/>
       </c>
-      <c r="M3" s="48">
+      <c r="M3" s="49">
         <f>L3-G3</f>
         <v/>
       </c>
-      <c r="N3" s="26">
+      <c r="N3" s="29">
         <f>M3/G3</f>
         <v/>
       </c>
-      <c r="O3" s="49" t="n">
+      <c r="O3" s="50" t="n">
         <v>43818</v>
       </c>
-      <c r="P3" s="50">
+      <c r="P3" s="51">
         <f>TODAY()-O3</f>
         <v/>
       </c>
-      <c r="Q3" s="52" t="inlineStr">
+      <c r="Q3" s="53" t="inlineStr">
         <is>
           <t>择时转换</t>
         </is>
@@ -1526,7 +1533,7 @@
       <c r="T3" s="0" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="8" t="inlineStr">
+      <c r="A4" s="9" t="inlineStr">
         <is>
           <t>001938</t>
         </is>
@@ -1541,52 +1548,52 @@
           <t>股票型</t>
         </is>
       </c>
-      <c r="D4" s="51" t="n">
+      <c r="D4" s="52" t="n">
         <v>0.38</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1.5811</v>
       </c>
-      <c r="F4" s="48" t="n">
+      <c r="F4" s="49" t="n">
         <v>7020.69</v>
       </c>
-      <c r="G4" s="48">
+      <c r="G4" s="49">
         <f>E4*F4</f>
         <v/>
       </c>
       <c r="H4" s="0" t="n">
-        <v>1.6824</v>
-      </c>
-      <c r="I4" s="0" t="n">
-        <v>1.6849</v>
-      </c>
-      <c r="J4" s="26" t="n">
-        <v>0.0015</v>
+        <v>1.6549</v>
+      </c>
+      <c r="I4" s="26" t="n">
+        <v>1.6403</v>
+      </c>
+      <c r="J4" s="27" t="n">
+        <v>-0.008800000000000001</v>
       </c>
       <c r="K4" s="27">
         <f>(I4-E4)/E4</f>
         <v/>
       </c>
-      <c r="L4" s="48">
+      <c r="L4" s="49">
         <f>H4*F4</f>
         <v/>
       </c>
-      <c r="M4" s="48">
+      <c r="M4" s="49">
         <f>L4-G4</f>
         <v/>
       </c>
-      <c r="N4" s="26">
+      <c r="N4" s="29">
         <f>M4/G4</f>
         <v/>
       </c>
-      <c r="O4" s="49" t="n">
+      <c r="O4" s="50" t="n">
         <v>43818</v>
       </c>
-      <c r="P4" s="50">
+      <c r="P4" s="51">
         <f>TODAY()-O4</f>
         <v/>
       </c>
-      <c r="Q4" s="52" t="inlineStr">
+      <c r="Q4" s="53" t="inlineStr">
         <is>
           <t>择时转换</t>
         </is>
@@ -1596,7 +1603,7 @@
       <c r="T4" s="0" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="8" t="inlineStr">
+      <c r="A5" s="9" t="inlineStr">
         <is>
           <t>001071</t>
         </is>
@@ -1611,52 +1618,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D5" s="47" t="n">
+      <c r="D5" s="48" t="n">
         <v>0.4</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1.9674</v>
       </c>
-      <c r="F5" s="48" t="n">
+      <c r="F5" s="49" t="n">
         <v>5388.05</v>
       </c>
-      <c r="G5" s="48">
+      <c r="G5" s="49">
         <f>E5*F5</f>
         <v/>
       </c>
       <c r="H5" s="0" t="n">
-        <v>2.102</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>2.0923</v>
-      </c>
-      <c r="J5" s="26" t="n">
-        <v>-0.0046</v>
+        <v>2.073</v>
+      </c>
+      <c r="I5" s="26" t="n">
+        <v>2.0335</v>
+      </c>
+      <c r="J5" s="27" t="n">
+        <v>-0.0191</v>
       </c>
       <c r="K5" s="27">
         <f>(I5-E5)/E5</f>
         <v/>
       </c>
-      <c r="L5" s="48">
+      <c r="L5" s="49">
         <f>H5*F5</f>
         <v/>
       </c>
-      <c r="M5" s="48">
+      <c r="M5" s="49">
         <f>L5-G5</f>
         <v/>
       </c>
-      <c r="N5" s="26">
+      <c r="N5" s="29">
         <f>M5/G5</f>
         <v/>
       </c>
-      <c r="O5" s="49" t="n">
+      <c r="O5" s="50" t="n">
         <v>43818</v>
       </c>
-      <c r="P5" s="50">
+      <c r="P5" s="51">
         <f>TODAY()-O5</f>
         <v/>
       </c>
-      <c r="Q5" s="48" t="inlineStr">
+      <c r="Q5" s="49" t="inlineStr">
         <is>
           <t>择时加仓</t>
         </is>
@@ -1666,7 +1673,7 @@
       <c r="T5" s="0" t="n"/>
     </row>
     <row r="6">
-      <c r="A6" s="8" t="inlineStr">
+      <c r="A6" s="9" t="inlineStr">
         <is>
           <t>006879</t>
         </is>
@@ -1681,52 +1688,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D6" s="48" t="n">
+      <c r="D6" s="49" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1.5817</v>
       </c>
-      <c r="F6" s="48" t="n">
+      <c r="F6" s="49" t="n">
         <v>6701.72</v>
       </c>
-      <c r="G6" s="48">
+      <c r="G6" s="49">
         <f>E6*F6</f>
         <v/>
       </c>
       <c r="H6" s="0" t="n">
-        <v>1.6905</v>
-      </c>
-      <c r="I6" s="0" t="n">
-        <v>1.6837</v>
-      </c>
-      <c r="J6" s="26" t="n">
-        <v>-0.004</v>
+        <v>1.6684</v>
+      </c>
+      <c r="I6" s="26" t="n">
+        <v>1.6371</v>
+      </c>
+      <c r="J6" s="27" t="n">
+        <v>-0.0188</v>
       </c>
       <c r="K6" s="27">
         <f>(I6-E6)/E6</f>
         <v/>
       </c>
-      <c r="L6" s="48">
+      <c r="L6" s="49">
         <f>H6*F6</f>
         <v/>
       </c>
-      <c r="M6" s="48">
+      <c r="M6" s="49">
         <f>L6-G6</f>
         <v/>
       </c>
-      <c r="N6" s="26">
+      <c r="N6" s="29">
         <f>M6/G6</f>
         <v/>
       </c>
-      <c r="O6" s="49" t="n">
+      <c r="O6" s="50" t="n">
         <v>43818</v>
       </c>
-      <c r="P6" s="50">
+      <c r="P6" s="51">
         <f>TODAY()-O6</f>
         <v/>
       </c>
-      <c r="Q6" s="48" t="inlineStr">
+      <c r="Q6" s="49" t="inlineStr">
         <is>
           <t>择时加仓</t>
         </is>
@@ -1736,7 +1743,7 @@
       <c r="T6" s="0" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="8" t="inlineStr">
+      <c r="A7" s="9" t="inlineStr">
         <is>
           <t>160225</t>
         </is>
@@ -1751,52 +1758,52 @@
           <t>指数型</t>
         </is>
       </c>
-      <c r="D7" s="53" t="n">
+      <c r="D7" s="54" t="n">
         <v>0.21</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>0.9862</v>
       </c>
-      <c r="F7" s="48" t="n">
+      <c r="F7" s="49" t="n">
         <v>12372.63</v>
       </c>
-      <c r="G7" s="48">
+      <c r="G7" s="49">
         <f>E7*F7</f>
         <v/>
       </c>
       <c r="H7" s="0" t="n">
-        <v>0.9877</v>
-      </c>
-      <c r="I7" s="0" t="n">
-        <v>0.9886</v>
-      </c>
-      <c r="J7" s="26" t="n">
-        <v>0.001</v>
+        <v>0.9864000000000001</v>
+      </c>
+      <c r="I7" s="26" t="n">
+        <v>0.9711</v>
+      </c>
+      <c r="J7" s="27" t="n">
+        <v>-0.0155</v>
       </c>
       <c r="K7" s="27">
         <f>(I7-E7)/E7</f>
         <v/>
       </c>
-      <c r="L7" s="48">
+      <c r="L7" s="49">
         <f>H7*F7</f>
         <v/>
       </c>
-      <c r="M7" s="48">
+      <c r="M7" s="49">
         <f>L7-G7</f>
         <v/>
       </c>
-      <c r="N7" s="26">
+      <c r="N7" s="29">
         <f>M7/G7</f>
         <v/>
       </c>
-      <c r="O7" s="49" t="n">
+      <c r="O7" s="50" t="n">
         <v>43843</v>
       </c>
-      <c r="P7" s="50">
+      <c r="P7" s="51">
         <f>TODAY()-O7</f>
         <v/>
       </c>
-      <c r="Q7" s="48" t="inlineStr">
+      <c r="Q7" s="49" t="inlineStr">
         <is>
           <t>择时逐步建仓</t>
         </is>
@@ -1806,7 +1813,7 @@
       <c r="T7" s="0" t="n"/>
     </row>
     <row r="8">
-      <c r="A8" s="8" t="inlineStr">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>007874</t>
         </is>
@@ -1821,52 +1828,52 @@
           <t>联接</t>
         </is>
       </c>
-      <c r="D8" s="48" t="n">
+      <c r="D8" s="49" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1.2629</v>
       </c>
-      <c r="F8" s="48" t="n">
+      <c r="F8" s="49" t="n">
         <v>5217.33</v>
       </c>
-      <c r="G8" s="48">
+      <c r="G8" s="49">
         <f>E8*F8</f>
         <v/>
       </c>
       <c r="H8" s="0" t="n">
-        <v>1.2725</v>
-      </c>
-      <c r="I8" s="0" t="n">
-        <v>1.2866</v>
-      </c>
-      <c r="J8" s="26" t="n">
-        <v>0.0111</v>
+        <v>1.2667</v>
+      </c>
+      <c r="I8" s="26" t="n">
+        <v>1.2609</v>
+      </c>
+      <c r="J8" s="27" t="n">
+        <v>-0.0046</v>
       </c>
       <c r="K8" s="27">
         <f>(I8-E8)/E8</f>
         <v/>
       </c>
-      <c r="L8" s="48">
+      <c r="L8" s="49">
         <f>H8*F8</f>
         <v/>
       </c>
-      <c r="M8" s="48">
+      <c r="M8" s="49">
         <f>L8-G8</f>
         <v/>
       </c>
-      <c r="N8" s="26">
+      <c r="N8" s="29">
         <f>M8/G8</f>
         <v/>
       </c>
-      <c r="O8" s="49" t="n">
+      <c r="O8" s="50" t="n">
         <v>43841</v>
       </c>
-      <c r="P8" s="50">
+      <c r="P8" s="51">
         <f>TODAY()-O8</f>
         <v/>
       </c>
-      <c r="Q8" s="48" t="inlineStr">
+      <c r="Q8" s="49" t="inlineStr">
         <is>
           <t>择时逐步建仓</t>
         </is>
@@ -1876,7 +1883,7 @@
       <c r="T8" s="0" t="n"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="inlineStr">
+      <c r="A9" s="4" t="inlineStr">
         <is>
           <t>005312</t>
         </is>
@@ -1895,44 +1902,44 @@
         <v>0.26</v>
       </c>
       <c r="E9" s="0" t="n">
-        <v>1.9208</v>
-      </c>
-      <c r="F9" s="48" t="n">
-        <v>5101.79</v>
-      </c>
-      <c r="G9" s="48">
+        <v>1.9096</v>
+      </c>
+      <c r="F9" s="49" t="n">
+        <v>5917.14</v>
+      </c>
+      <c r="G9" s="49">
         <f>F9*E9</f>
         <v/>
       </c>
       <c r="H9" s="0" t="n">
-        <v>1.7627</v>
-      </c>
-      <c r="I9" s="54" t="n">
-        <v>1.7951</v>
-      </c>
-      <c r="J9" s="29" t="n">
-        <v>0.0184</v>
+        <v>1.7556</v>
+      </c>
+      <c r="I9" s="26" t="n">
+        <v>1.7761</v>
+      </c>
+      <c r="J9" s="27" t="n">
+        <v>0.0117</v>
       </c>
       <c r="K9" s="27">
         <f>(I9-E9)/E9</f>
         <v/>
       </c>
-      <c r="L9" s="48">
+      <c r="L9" s="49">
         <f>H9*F9</f>
         <v/>
       </c>
-      <c r="M9" s="48">
+      <c r="M9" s="49">
         <f>L9-G9</f>
         <v/>
       </c>
-      <c r="N9" s="26">
+      <c r="N9" s="29">
         <f>M9/G9</f>
         <v/>
       </c>
-      <c r="O9" s="49" t="n">
+      <c r="O9" s="50" t="n">
         <v>43878</v>
       </c>
-      <c r="P9" s="34">
+      <c r="P9" s="35">
         <f>TODAY()-O9</f>
         <v/>
       </c>
@@ -1942,7 +1949,7 @@
       <c r="T9" s="0" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="inlineStr">
+      <c r="A10" s="9" t="inlineStr">
         <is>
           <t>008087</t>
         </is>
@@ -1957,63 +1964,63 @@
           <t>联接</t>
         </is>
       </c>
-      <c r="D10" s="48" t="n">
+      <c r="D10" s="49" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>1.2232</v>
-      </c>
-      <c r="F10" s="48" t="n">
-        <v>989.21</v>
-      </c>
-      <c r="G10" s="48">
+        <v>1.2037</v>
+      </c>
+      <c r="F10" s="49" t="n">
+        <v>1420.73</v>
+      </c>
+      <c r="G10" s="49">
         <f>F10*E10</f>
         <v/>
       </c>
       <c r="H10" s="0" t="n">
-        <v>1.1587</v>
-      </c>
-      <c r="I10" s="54" t="n">
-        <v>1.176</v>
-      </c>
-      <c r="J10" s="29" t="n">
-        <v>0.0149</v>
+        <v>1.1813</v>
+      </c>
+      <c r="I10" s="26" t="n">
+        <v>1.1801</v>
+      </c>
+      <c r="J10" s="27" t="n">
+        <v>-0.001</v>
       </c>
       <c r="K10" s="27">
         <f>(I10-E10)/E10</f>
         <v/>
       </c>
-      <c r="L10" s="48">
+      <c r="L10" s="49">
         <f>H10*F10</f>
         <v/>
       </c>
-      <c r="M10" s="48">
+      <c r="M10" s="49">
         <f>L10-G10</f>
         <v/>
       </c>
-      <c r="N10" s="26">
+      <c r="N10" s="29">
         <f>M10/G10</f>
         <v/>
       </c>
-      <c r="O10" s="49" t="n">
+      <c r="O10" s="50" t="n">
         <v>43894</v>
       </c>
-      <c r="P10" s="34">
+      <c r="P10" s="35">
         <f>TODAY()-O10</f>
         <v/>
       </c>
-      <c r="Q10" s="52" t="n"/>
+      <c r="Q10" s="53" t="n"/>
       <c r="R10" s="0" t="n"/>
       <c r="S10" s="0" t="n"/>
       <c r="T10" s="0" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="11" s="9">
-      <c r="A11" s="3" t="inlineStr">
+    <row customHeight="1" ht="15.75" r="11" s="1">
+      <c r="A11" s="4" t="inlineStr">
         <is>
           <t>005963</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="5" t="inlineStr">
         <is>
           <t>宝盈人工智能股票C</t>
         </is>
@@ -2027,44 +2034,44 @@
         <v>0.35</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2.0811</v>
-      </c>
-      <c r="F11" s="48" t="n">
-        <v>1922.14</v>
-      </c>
-      <c r="G11" s="48">
+        <v>2.0614</v>
+      </c>
+      <c r="F11" s="49" t="n">
+        <v>2183.02</v>
+      </c>
+      <c r="G11" s="49">
         <f>F11*E11</f>
         <v/>
       </c>
       <c r="H11" s="0" t="n">
-        <v>1.9166</v>
-      </c>
-      <c r="I11" s="54" t="n">
-        <v>1.9306</v>
-      </c>
-      <c r="J11" s="29" t="n">
-        <v>0.0073</v>
+        <v>1.88</v>
+      </c>
+      <c r="I11" s="26" t="n">
+        <v>1.8742</v>
+      </c>
+      <c r="J11" s="27" t="n">
+        <v>-0.0031</v>
       </c>
       <c r="K11" s="27">
         <f>(I11-E11)/E11</f>
         <v/>
       </c>
-      <c r="L11" s="48">
+      <c r="L11" s="49">
         <f>H11*F11</f>
         <v/>
       </c>
-      <c r="M11" s="48">
+      <c r="M11" s="49">
         <f>L11-G11</f>
         <v/>
       </c>
-      <c r="N11" s="26">
+      <c r="N11" s="29">
         <f>M11/G11</f>
         <v/>
       </c>
-      <c r="O11" s="49" t="n">
+      <c r="O11" s="50" t="n">
         <v>43887</v>
       </c>
-      <c r="P11" s="34">
+      <c r="P11" s="35">
         <f>TODAY()-O11</f>
         <v/>
       </c>
@@ -2074,7 +2081,7 @@
       <c r="T11" s="0" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="inlineStr">
+      <c r="A12" s="9" t="inlineStr">
         <is>
           <t>003511</t>
         </is>
@@ -2089,52 +2096,52 @@
           <t>债券型</t>
         </is>
       </c>
-      <c r="D12" s="53" t="n">
+      <c r="D12" s="54" t="n">
         <v>0.28</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1.2202</v>
       </c>
-      <c r="F12" s="48" t="n">
+      <c r="F12" s="49" t="n">
         <v>4002</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="49">
         <f>E12*F12</f>
         <v/>
       </c>
       <c r="H12" s="0" t="n">
-        <v>1.2749</v>
-      </c>
-      <c r="I12" s="0" t="n">
-        <v>1.2753</v>
-      </c>
-      <c r="J12" s="26" t="n">
-        <v>0.0003</v>
+        <v>1.2708</v>
+      </c>
+      <c r="I12" s="26" t="n">
+        <v>1.2596</v>
+      </c>
+      <c r="J12" s="27" t="n">
+        <v>-0.008800000000000001</v>
       </c>
       <c r="K12" s="27">
         <f>(I12-E12)/E12</f>
         <v/>
       </c>
-      <c r="L12" s="48">
+      <c r="L12" s="49">
         <f>H12*F12</f>
         <v/>
       </c>
-      <c r="M12" s="48">
+      <c r="M12" s="49">
         <f>L12-G12</f>
         <v/>
       </c>
-      <c r="N12" s="26">
+      <c r="N12" s="29">
         <f>M12/G12</f>
         <v/>
       </c>
-      <c r="O12" s="49" t="n">
+      <c r="O12" s="50" t="n">
         <v>43838</v>
       </c>
-      <c r="P12" s="50">
+      <c r="P12" s="51">
         <f>TODAY()-O12</f>
         <v/>
       </c>
-      <c r="Q12" s="48" t="inlineStr">
+      <c r="Q12" s="49" t="inlineStr">
         <is>
           <t>择时逐步建仓</t>
         </is>
@@ -2144,7 +2151,7 @@
       <c r="T12" s="0" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="inlineStr">
+      <c r="A13" s="9" t="inlineStr">
         <is>
           <t>399001</t>
         </is>
@@ -2159,52 +2166,52 @@
           <t>指数型</t>
         </is>
       </c>
-      <c r="D13" s="53" t="n">
+      <c r="D13" s="54" t="n">
         <v>0.17</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1.3539</v>
       </c>
-      <c r="F13" s="48" t="n">
+      <c r="F13" s="49" t="n">
         <v>5871.94</v>
       </c>
-      <c r="G13" s="48">
+      <c r="G13" s="49">
         <f>E13*F13</f>
         <v/>
       </c>
       <c r="H13" s="0" t="n">
-        <v>1.346</v>
-      </c>
-      <c r="I13" s="54" t="n">
-        <v>1.3547</v>
-      </c>
-      <c r="J13" s="26" t="n">
-        <v>0.006500000000000001</v>
+        <v>1.335</v>
+      </c>
+      <c r="I13" s="26" t="n">
+        <v>1.3157</v>
+      </c>
+      <c r="J13" s="27" t="n">
+        <v>-0.0144</v>
       </c>
       <c r="K13" s="27">
         <f>(I13-E13)/E13</f>
         <v/>
       </c>
-      <c r="L13" s="48">
+      <c r="L13" s="49">
         <f>H13*F13</f>
         <v/>
       </c>
-      <c r="M13" s="48">
+      <c r="M13" s="49">
         <f>L13-G13</f>
         <v/>
       </c>
-      <c r="N13" s="26">
+      <c r="N13" s="29">
         <f>M13/G13</f>
         <v/>
       </c>
-      <c r="O13" s="49" t="n">
+      <c r="O13" s="50" t="n">
         <v>43834</v>
       </c>
-      <c r="P13" s="50">
+      <c r="P13" s="51">
         <f>TODAY()-O13</f>
         <v/>
       </c>
-      <c r="Q13" s="52" t="inlineStr">
+      <c r="Q13" s="53" t="inlineStr">
         <is>
           <t>找机会转出清仓</t>
         </is>
@@ -2214,7 +2221,7 @@
       <c r="T13" s="0" t="n"/>
     </row>
     <row r="14">
-      <c r="A14" s="8" t="inlineStr">
+      <c r="A14" s="9" t="inlineStr">
         <is>
           <t>110003</t>
         </is>
@@ -2229,52 +2236,52 @@
           <t>指数型</t>
         </is>
       </c>
-      <c r="D14" s="53" t="n">
+      <c r="D14" s="54" t="n">
         <v>0.25</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1.7618</v>
       </c>
-      <c r="F14" s="48" t="n">
+      <c r="F14" s="49" t="n">
         <v>1305.5</v>
       </c>
-      <c r="G14" s="48">
+      <c r="G14" s="49">
         <f>E14*F14</f>
         <v/>
       </c>
       <c r="H14" s="0" t="n">
-        <v>1.7307</v>
-      </c>
-      <c r="I14" s="54" t="n">
-        <v>1.7419</v>
-      </c>
-      <c r="J14" s="26" t="n">
-        <v>0.006500000000000001</v>
+        <v>1.7116</v>
+      </c>
+      <c r="I14" s="26" t="n">
+        <v>1.6869</v>
+      </c>
+      <c r="J14" s="27" t="n">
+        <v>-0.0144</v>
       </c>
       <c r="K14" s="27">
         <f>(I14-E14)/E14</f>
         <v/>
       </c>
-      <c r="L14" s="48">
+      <c r="L14" s="49">
         <f>H14*F14</f>
         <v/>
       </c>
-      <c r="M14" s="48">
+      <c r="M14" s="49">
         <f>L14-G14</f>
         <v/>
       </c>
-      <c r="N14" s="26">
+      <c r="N14" s="29">
         <f>M14/G14</f>
         <v/>
       </c>
-      <c r="O14" s="49" t="n">
+      <c r="O14" s="50" t="n">
         <v>43837</v>
       </c>
-      <c r="P14" s="50">
+      <c r="P14" s="51">
         <f>TODAY()-O14</f>
         <v/>
       </c>
-      <c r="Q14" s="52" t="inlineStr">
+      <c r="Q14" s="53" t="inlineStr">
         <is>
           <t>找机会转出清仓</t>
         </is>
@@ -2284,7 +2291,7 @@
       <c r="T14" s="0" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="8" t="inlineStr">
+      <c r="A15" s="9" t="inlineStr">
         <is>
           <t>000083</t>
         </is>
@@ -2299,52 +2306,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D15" s="51" t="n">
+      <c r="D15" s="52" t="n">
         <v>0.36</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>4.6851</v>
       </c>
-      <c r="F15" s="48" t="n">
+      <c r="F15" s="49" t="n">
         <v>1227.32</v>
       </c>
-      <c r="G15" s="48">
+      <c r="G15" s="49">
         <f>E15*F15</f>
         <v/>
       </c>
       <c r="H15" s="0" t="n">
-        <v>4.789</v>
-      </c>
-      <c r="I15" s="0" t="n">
-        <v>4.8136</v>
-      </c>
-      <c r="J15" s="26" t="n">
-        <v>0.0051</v>
+        <v>4.759</v>
+      </c>
+      <c r="I15" s="26" t="n">
+        <v>4.6884</v>
+      </c>
+      <c r="J15" s="27" t="n">
+        <v>-0.0148</v>
       </c>
       <c r="K15" s="27">
         <f>(I15-E15)/E15</f>
         <v/>
       </c>
-      <c r="L15" s="48">
+      <c r="L15" s="49">
         <f>H15*F15</f>
         <v/>
       </c>
-      <c r="M15" s="48">
+      <c r="M15" s="49">
         <f>L15-G15</f>
         <v/>
       </c>
-      <c r="N15" s="26">
+      <c r="N15" s="29">
         <f>M15/G15</f>
         <v/>
       </c>
-      <c r="O15" s="49" t="n">
+      <c r="O15" s="50" t="n">
         <v>43831</v>
       </c>
-      <c r="P15" s="50">
+      <c r="P15" s="51">
         <f>TODAY()-O15</f>
         <v/>
       </c>
-      <c r="Q15" s="48" t="inlineStr">
+      <c r="Q15" s="49" t="inlineStr">
         <is>
           <t>择时逐步建仓</t>
         </is>
@@ -2354,7 +2361,7 @@
       <c r="T15" s="0" t="n"/>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="inlineStr">
+      <c r="A16" s="9" t="inlineStr">
         <is>
           <t>519778</t>
         </is>
@@ -2369,52 +2376,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D16" s="47" t="n">
+      <c r="D16" s="48" t="n">
         <v>0.45</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>2.0642</v>
       </c>
-      <c r="F16" s="48" t="n">
+      <c r="F16" s="49" t="n">
         <v>290.67</v>
       </c>
-      <c r="G16" s="48">
+      <c r="G16" s="49">
         <f>E16*F16</f>
         <v/>
       </c>
       <c r="H16" s="0" t="n">
-        <v>2.2416</v>
-      </c>
-      <c r="I16" s="0" t="n">
-        <v>2.2615</v>
-      </c>
-      <c r="J16" s="26" t="n">
-        <v>0.0089</v>
+        <v>2.2106</v>
+      </c>
+      <c r="I16" s="26" t="n">
+        <v>2.1902</v>
+      </c>
+      <c r="J16" s="27" t="n">
+        <v>-0.0092</v>
       </c>
       <c r="K16" s="27">
         <f>(I16-E16)/E16</f>
         <v/>
       </c>
-      <c r="L16" s="48">
+      <c r="L16" s="49">
         <f>H16*F16</f>
         <v/>
       </c>
-      <c r="M16" s="48">
+      <c r="M16" s="49">
         <f>L16-G16</f>
         <v/>
       </c>
-      <c r="N16" s="26">
+      <c r="N16" s="29">
         <f>M16/G16</f>
         <v/>
       </c>
-      <c r="O16" s="49" t="n">
+      <c r="O16" s="50" t="n">
         <v>43838</v>
       </c>
-      <c r="P16" s="50">
+      <c r="P16" s="51">
         <f>TODAY()-O16</f>
         <v/>
       </c>
-      <c r="Q16" s="48" t="inlineStr">
+      <c r="Q16" s="49" t="inlineStr">
         <is>
           <t>择时建仓</t>
         </is>
@@ -2424,7 +2431,7 @@
       <c r="T16" s="0" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="inlineStr">
+      <c r="A17" s="9" t="inlineStr">
         <is>
           <t>008507</t>
         </is>
@@ -2439,52 +2446,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D17" s="48" t="n">
+      <c r="D17" s="49" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="0" t="n">
         <v>1.0535</v>
       </c>
-      <c r="F17" s="48" t="n">
+      <c r="F17" s="49" t="n">
         <v>1909.04</v>
       </c>
-      <c r="G17" s="48">
+      <c r="G17" s="49">
         <f>E17*F17</f>
         <v/>
       </c>
       <c r="H17" s="0" t="n">
-        <v>1.0257</v>
-      </c>
-      <c r="I17" s="54" t="n">
-        <v>1.0249</v>
-      </c>
-      <c r="J17" s="26" t="n">
-        <v>-0.0008</v>
+        <v>1.0154</v>
+      </c>
+      <c r="I17" s="26" t="n">
+        <v>1.0108</v>
+      </c>
+      <c r="J17" s="27" t="n">
+        <v>-0.004500000000000001</v>
       </c>
       <c r="K17" s="27">
         <f>(I17-E17)/E17</f>
         <v/>
       </c>
-      <c r="L17" s="48">
+      <c r="L17" s="49">
         <f>H17*F17</f>
         <v/>
       </c>
-      <c r="M17" s="48">
+      <c r="M17" s="49">
         <f>L17-G17</f>
         <v/>
       </c>
-      <c r="N17" s="26">
+      <c r="N17" s="29">
         <f>M17/G17</f>
         <v/>
       </c>
-      <c r="O17" s="49" t="n">
+      <c r="O17" s="50" t="n">
         <v>43838</v>
       </c>
-      <c r="P17" s="50">
+      <c r="P17" s="51">
         <f>TODAY()-O17</f>
         <v/>
       </c>
-      <c r="Q17" s="48" t="inlineStr">
+      <c r="Q17" s="49" t="inlineStr">
         <is>
           <t>择时逐步建仓</t>
         </is>
@@ -2494,7 +2501,7 @@
       <c r="T17" s="0" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="44" t="inlineStr">
+      <c r="A18" s="45" t="inlineStr">
         <is>
           <t>008638</t>
         </is>
@@ -2509,52 +2516,52 @@
           <t>混合型</t>
         </is>
       </c>
-      <c r="D18" s="48" t="n">
+      <c r="D18" s="49" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="0" t="n">
         <v>1.0013</v>
       </c>
-      <c r="F18" s="48" t="n">
+      <c r="F18" s="49" t="n">
         <v>329.41</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="49">
         <f>E18*F18</f>
         <v/>
       </c>
       <c r="H18" s="0" t="n">
-        <v>1.0671</v>
-      </c>
-      <c r="I18" s="0" t="n">
-        <v>1.0679</v>
-      </c>
-      <c r="J18" s="26" t="n">
-        <v>0.0007000000000000001</v>
+        <v>1.051</v>
+      </c>
+      <c r="I18" s="26" t="n">
+        <v>1.0465</v>
+      </c>
+      <c r="J18" s="27" t="n">
+        <v>-0.0043</v>
       </c>
       <c r="K18" s="27">
         <f>(I18-E18)/E18</f>
         <v/>
       </c>
-      <c r="L18" s="48">
+      <c r="L18" s="49">
         <f>H18*F18</f>
         <v/>
       </c>
-      <c r="M18" s="48">
+      <c r="M18" s="49">
         <f>L18-G18</f>
         <v/>
       </c>
-      <c r="N18" s="26">
+      <c r="N18" s="29">
         <f>M18/G18</f>
         <v/>
       </c>
-      <c r="O18" s="49" t="n">
+      <c r="O18" s="50" t="n">
         <v>43819</v>
       </c>
-      <c r="P18" s="50">
+      <c r="P18" s="51">
         <f>TODAY()-O18</f>
         <v/>
       </c>
-      <c r="Q18" s="48" t="inlineStr">
+      <c r="Q18" s="49" t="inlineStr">
         <is>
           <t>择时加仓</t>
         </is>
@@ -2564,12 +2571,12 @@
       <c r="T18" s="0" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="inlineStr">
+      <c r="A19" s="4" t="inlineStr">
         <is>
           <t>000404</t>
         </is>
       </c>
-      <c r="B19" s="5" t="inlineStr">
+      <c r="B19" s="6" t="inlineStr">
         <is>
           <t>易方达新兴成长灵活配置</t>
         </is>
@@ -2583,44 +2590,44 @@
         <v>0.41</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>3.5568</v>
-      </c>
-      <c r="F19" s="48" t="n">
-        <v>1851.81</v>
-      </c>
-      <c r="G19" s="48">
+        <v>3.5394</v>
+      </c>
+      <c r="F19" s="49" t="n">
+        <v>2002.19</v>
+      </c>
+      <c r="G19" s="49">
         <f>F19*E19</f>
         <v/>
       </c>
       <c r="H19" s="0" t="n">
-        <v>3.32</v>
-      </c>
-      <c r="I19" s="54" t="n">
-        <v>3.3323</v>
-      </c>
-      <c r="J19" s="29" t="n">
-        <v>0.0037</v>
+        <v>3.255</v>
+      </c>
+      <c r="I19" s="26" t="n">
+        <v>3.2127</v>
+      </c>
+      <c r="J19" s="27" t="n">
+        <v>-0.013</v>
       </c>
       <c r="K19" s="27">
         <f>(I19-E19)/E19</f>
         <v/>
       </c>
-      <c r="L19" s="48">
+      <c r="L19" s="49">
         <f>H19*F19</f>
         <v/>
       </c>
-      <c r="M19" s="48">
+      <c r="M19" s="49">
         <f>L19-G19</f>
         <v/>
       </c>
-      <c r="N19" s="26">
+      <c r="N19" s="29">
         <f>M19/G19</f>
         <v/>
       </c>
-      <c r="O19" s="49" t="n">
+      <c r="O19" s="50" t="n">
         <v>43880</v>
       </c>
-      <c r="P19" s="34">
+      <c r="P19" s="35">
         <f>TODAY()-O19</f>
         <v/>
       </c>
@@ -2645,27 +2652,27 @@
           <t>联接</t>
         </is>
       </c>
-      <c r="D20" s="53" t="n">
+      <c r="D20" s="54" t="n">
         <v>0.19</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1.0732</v>
       </c>
-      <c r="F20" s="48" t="n">
+      <c r="F20" s="49" t="n">
         <v>22838.46</v>
       </c>
-      <c r="G20" s="48">
+      <c r="G20" s="49">
         <f>E20*F20</f>
         <v/>
       </c>
       <c r="H20" s="0" t="n">
-        <v>1.0822</v>
-      </c>
-      <c r="I20" s="0" t="n">
-        <v>1.0854</v>
-      </c>
-      <c r="J20" s="26" t="n">
-        <v>0.0029</v>
+        <v>1.0701</v>
+      </c>
+      <c r="I20" s="26" t="n">
+        <v>1.0558</v>
+      </c>
+      <c r="J20" s="27" t="n">
+        <v>-0.0134</v>
       </c>
       <c r="K20" s="27">
         <f>(I20-E20)/E20</f>
@@ -2679,24 +2686,24 @@
         <f>L20-G20</f>
         <v/>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="28">
         <f>M20/G20</f>
         <v/>
       </c>
-      <c r="O20" s="35" t="n">
+      <c r="O20" s="36" t="n">
         <v>43728</v>
       </c>
       <c r="P20" s="56">
         <f>TODAY()-O20</f>
         <v/>
       </c>
-      <c r="Q20" s="48" t="n"/>
+      <c r="Q20" s="49" t="n"/>
       <c r="R20" s="0" t="n"/>
       <c r="S20" s="0" t="n"/>
       <c r="T20" s="0" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="8" t="inlineStr">
+      <c r="A21" s="9" t="inlineStr">
         <is>
           <t>270042</t>
         </is>
@@ -2711,62 +2718,62 @@
           <t>QDII-指数</t>
         </is>
       </c>
-      <c r="D21" s="47" t="n">
+      <c r="D21" s="48" t="n">
         <v>0.4</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>2.8237</v>
       </c>
-      <c r="F21" s="48" t="n">
+      <c r="F21" s="49" t="n">
         <v>1012.86</v>
       </c>
-      <c r="G21" s="48">
+      <c r="G21" s="49">
         <f>E21*F21</f>
         <v/>
       </c>
       <c r="H21" s="0" t="n">
-        <v>2.6413</v>
-      </c>
-      <c r="I21" s="54" t="n">
-        <v>2.4584</v>
-      </c>
-      <c r="J21" s="29" t="n">
-        <v>-0.0692</v>
+        <v>2.4846</v>
+      </c>
+      <c r="I21" s="26" t="n">
+        <v>2.2619</v>
+      </c>
+      <c r="J21" s="27" t="n">
+        <v>-0.08960000000000001</v>
       </c>
       <c r="K21" s="27">
         <f>(I21-E21)/E21</f>
         <v/>
       </c>
-      <c r="L21" s="48">
+      <c r="L21" s="49">
         <f>H21*F21</f>
         <v/>
       </c>
-      <c r="M21" s="48">
+      <c r="M21" s="49">
         <f>L21-G21</f>
         <v/>
       </c>
-      <c r="N21" s="26">
+      <c r="N21" s="29">
         <f>M21/G21</f>
         <v/>
       </c>
-      <c r="O21" s="49" t="n">
+      <c r="O21" s="50" t="n">
         <v>43825</v>
       </c>
-      <c r="P21" s="50">
+      <c r="P21" s="51">
         <f>TODAY()-O21</f>
         <v/>
       </c>
-      <c r="Q21" s="48" t="inlineStr">
+      <c r="Q21" s="49" t="inlineStr">
         <is>
           <t>定投</t>
         </is>
       </c>
-      <c r="R21" s="8" t="n"/>
-      <c r="S21" s="8" t="n"/>
+      <c r="R21" s="9" t="n"/>
+      <c r="S21" s="9" t="n"/>
       <c r="T21" s="0" t="n"/>
     </row>
     <row r="22">
-      <c r="A22" s="8" t="inlineStr">
+      <c r="A22" s="9" t="inlineStr">
         <is>
           <t>161128</t>
         </is>
@@ -2781,85 +2788,85 @@
           <t>QDII-指数</t>
         </is>
       </c>
-      <c r="D22" s="47" t="n">
+      <c r="D22" s="48" t="n">
         <v>0.45</v>
       </c>
       <c r="E22" s="0" t="n">
         <v>1.8642</v>
       </c>
-      <c r="F22" s="48" t="n">
+      <c r="F22" s="49" t="n">
         <v>2092.12</v>
       </c>
-      <c r="G22" s="48">
+      <c r="G22" s="49">
         <f>E22*F22</f>
         <v/>
       </c>
       <c r="H22" s="0" t="n">
-        <v>1.7482</v>
-      </c>
-      <c r="I22" s="54" t="n">
-        <v>1.6236</v>
-      </c>
-      <c r="J22" s="29" t="n">
-        <v>-0.0713</v>
+        <v>1.6474</v>
+      </c>
+      <c r="I22" s="26" t="n">
+        <v>1.4904</v>
+      </c>
+      <c r="J22" s="27" t="n">
+        <v>-0.0953</v>
       </c>
       <c r="K22" s="27">
         <f>(I22-E22)/E22</f>
         <v/>
       </c>
-      <c r="L22" s="48">
+      <c r="L22" s="49">
         <f>H22*F22</f>
         <v/>
       </c>
-      <c r="M22" s="48">
+      <c r="M22" s="49">
         <f>L22-G22</f>
         <v/>
       </c>
-      <c r="N22" s="26">
+      <c r="N22" s="29">
         <f>M22/G22</f>
         <v/>
       </c>
-      <c r="O22" s="49" t="n">
+      <c r="O22" s="50" t="n">
         <v>43824</v>
       </c>
-      <c r="P22" s="50">
+      <c r="P22" s="51">
         <f>TODAY()-O22</f>
         <v/>
       </c>
-      <c r="Q22" s="48" t="inlineStr">
+      <c r="Q22" s="49" t="inlineStr">
         <is>
           <t>定投</t>
         </is>
       </c>
-      <c r="R22" s="8" t="n"/>
-      <c r="S22" s="8" t="n"/>
+      <c r="R22" s="9" t="n"/>
+      <c r="S22" s="9" t="n"/>
       <c r="T22" s="0" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="0" t="n"/>
       <c r="B23" s="0" t="n"/>
       <c r="E23" s="57" t="n"/>
-      <c r="F23" s="48" t="n"/>
-      <c r="G23" s="48" t="n"/>
+      <c r="F23" s="49" t="n"/>
+      <c r="G23" s="49" t="n"/>
       <c r="H23" s="57" t="n"/>
       <c r="I23" s="57" t="n"/>
       <c r="J23" s="57" t="n"/>
       <c r="K23" s="57" t="n"/>
-      <c r="L23" s="48" t="n"/>
-      <c r="M23" s="48" t="n"/>
-      <c r="N23" s="48">
+      <c r="L23" s="49" t="n"/>
+      <c r="M23" s="49" t="n"/>
+      <c r="N23" s="49">
         <f>M23*0.5/100</f>
         <v/>
       </c>
-      <c r="O23" s="49" t="n"/>
-      <c r="P23" s="26" t="n"/>
-      <c r="Q23" s="48" t="n"/>
+      <c r="O23" s="50" t="n"/>
+      <c r="P23" s="29" t="n"/>
+      <c r="Q23" s="49" t="n"/>
       <c r="R23" s="0" t="n"/>
       <c r="S23" s="0" t="n"/>
       <c r="T23" s="0" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="8" t="inlineStr">
+      <c r="A24" s="9" t="inlineStr">
         <is>
           <t>基金数量</t>
         </is>
@@ -2868,14 +2875,14 @@
         <f>COUNTA(B2:B20)</f>
         <v/>
       </c>
-      <c r="D24" s="48" t="n"/>
+      <c r="D24" s="49" t="n"/>
       <c r="E24" s="57" t="n"/>
-      <c r="F24" s="48" t="inlineStr">
+      <c r="F24" s="49" t="inlineStr">
         <is>
           <t>总成本</t>
         </is>
       </c>
-      <c r="G24" s="48">
+      <c r="G24" s="49">
         <f>SUM(G2:G20)</f>
         <v/>
       </c>
@@ -2883,22 +2890,22 @@
       <c r="I24" s="57" t="n"/>
       <c r="J24" s="57" t="n"/>
       <c r="K24" s="57" t="n"/>
-      <c r="L24" s="48" t="inlineStr">
+      <c r="L24" s="49" t="inlineStr">
         <is>
           <t>总收益</t>
         </is>
       </c>
-      <c r="M24" s="48">
+      <c r="M24" s="49">
         <f>SUM(M2:M20)</f>
         <v/>
       </c>
-      <c r="N24" s="26">
+      <c r="N24" s="29">
         <f>M24/G24</f>
         <v/>
       </c>
       <c r="O24" s="58" t="n"/>
       <c r="P24" s="59" t="n"/>
-      <c r="Q24" s="52" t="n"/>
+      <c r="Q24" s="53" t="n"/>
       <c r="R24" s="0" t="n"/>
       <c r="S24" s="0" t="n"/>
       <c r="T24" s="0" t="n"/>
@@ -2922,7 +2929,7 @@
           <t>国联安中证半导体ETF联接C</t>
         </is>
       </c>
-      <c r="C31" s="7" t="inlineStr">
+      <c r="C31" s="8" t="inlineStr">
         <is>
           <t>联接</t>
         </is>
@@ -2930,7 +2937,7 @@
       <c r="D31" s="55" t="n">
         <v>0</v>
       </c>
-      <c r="E31" s="7" t="n">
+      <c r="E31" s="8" t="n">
         <v>1.7717</v>
       </c>
       <c r="F31" s="55">
@@ -2941,16 +2948,16 @@
         <f>E31*F31</f>
         <v/>
       </c>
-      <c r="H31" s="7" t="n">
+      <c r="H31" s="8" t="n">
         <v>1.9334</v>
       </c>
-      <c r="I31" s="7" t="n">
+      <c r="I31" s="8" t="n">
         <v>1.906</v>
       </c>
-      <c r="J31" s="30" t="n">
+      <c r="J31" s="28" t="n">
         <v>-0.0142</v>
       </c>
-      <c r="K31" s="26">
+      <c r="K31" s="29">
         <f>(I31-E31)/E31</f>
         <v/>
       </c>
@@ -2962,7 +2969,7 @@
         <f>L31-G31</f>
         <v/>
       </c>
-      <c r="N31" s="30">
+      <c r="N31" s="28">
         <f>M31/G31</f>
         <v/>
       </c>
@@ -2978,26 +2985,26 @@
           <t>已卖出清仓</t>
         </is>
       </c>
-      <c r="R31" s="42" t="n">
+      <c r="R31" s="43" t="n">
         <v>43893</v>
       </c>
-      <c r="S31" s="7" t="n">
+      <c r="S31" s="8" t="n">
         <v>113</v>
       </c>
       <c r="T31" s="0" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="6" t="inlineStr">
+      <c r="A32" s="7" t="inlineStr">
         <is>
           <t>161028</t>
         </is>
       </c>
-      <c r="B32" s="7" t="inlineStr">
+      <c r="B32" s="8" t="inlineStr">
         <is>
           <t>富国中征信能源汽车指数分级</t>
         </is>
       </c>
-      <c r="C32" s="7" t="inlineStr">
+      <c r="C32" s="8" t="inlineStr">
         <is>
           <t>指数型</t>
         </is>
@@ -3005,26 +3012,26 @@
       <c r="D32" s="55" t="n">
         <v>0.29</v>
       </c>
-      <c r="E32" s="7" t="n">
-        <v>2.6863</v>
+      <c r="E32" s="8" t="n">
+        <v>1.2084</v>
       </c>
       <c r="F32" s="55" t="n">
-        <v>20.62</v>
+        <v>128.6</v>
       </c>
       <c r="G32" s="55">
         <f>E32*F32</f>
         <v/>
       </c>
-      <c r="H32" s="7" t="n">
-        <v>0.925</v>
-      </c>
-      <c r="I32" s="62" t="n">
-        <v>0.9223</v>
+      <c r="H32" s="8" t="n">
+        <v>0.901</v>
+      </c>
+      <c r="I32" s="30" t="n">
+        <v>0.8807</v>
       </c>
       <c r="J32" s="31" t="n">
-        <v>-0.0029</v>
-      </c>
-      <c r="K32" s="26">
+        <v>-0.0226</v>
+      </c>
+      <c r="K32" s="29">
         <f>(I32-E32)/E32</f>
         <v/>
       </c>
@@ -3036,7 +3043,7 @@
         <f>L32-G32</f>
         <v/>
       </c>
-      <c r="N32" s="30">
+      <c r="N32" s="28">
         <f>M32/G32</f>
         <v/>
       </c>
@@ -3047,25 +3054,25 @@
         <f>TODAY()-O32</f>
         <v/>
       </c>
-      <c r="Q32" s="63" t="inlineStr">
+      <c r="Q32" s="62" t="inlineStr">
         <is>
           <t>已卖出清仓，没赚到</t>
         </is>
       </c>
-      <c r="R32" s="7" t="n">
+      <c r="R32" s="8" t="n">
         <v>43893</v>
       </c>
-      <c r="S32" s="7" t="n"/>
+      <c r="S32" s="8" t="n"/>
       <c r="T32" s="0" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="6" t="n"/>
-      <c r="B33" s="7" t="inlineStr">
+      <c r="A33" s="7" t="n"/>
+      <c r="B33" s="8" t="inlineStr">
         <is>
           <t>工银金融地产混合</t>
         </is>
       </c>
-      <c r="C33" s="7" t="inlineStr">
+      <c r="C33" s="8" t="inlineStr">
         <is>
           <t>混合型</t>
         </is>
@@ -3073,7 +3080,7 @@
       <c r="D33" s="55" t="n">
         <v>0.18</v>
       </c>
-      <c r="E33" s="7" t="n">
+      <c r="E33" s="8" t="n">
         <v>2.2495</v>
       </c>
       <c r="F33" s="55" t="n">
@@ -3083,16 +3090,16 @@
         <f>E33*F33</f>
         <v/>
       </c>
-      <c r="H33" s="7" t="n">
+      <c r="H33" s="8" t="n">
         <v>2.269</v>
       </c>
       <c r="I33" s="22" t="n">
         <v>2.2307</v>
       </c>
-      <c r="J33" s="31" t="n">
+      <c r="J33" s="32" t="n">
         <v>-0.0169</v>
       </c>
-      <c r="K33" s="26">
+      <c r="K33" s="29">
         <f>(I33-E33)/E33</f>
         <v/>
       </c>
@@ -3104,7 +3111,7 @@
         <f>L33-G33</f>
         <v/>
       </c>
-      <c r="N33" s="30">
+      <c r="N33" s="28">
         <f>M33/G33</f>
         <v/>
       </c>
@@ -3115,17 +3122,17 @@
         <f>TODAY()-O33</f>
         <v/>
       </c>
-      <c r="Q33" s="63" t="inlineStr">
+      <c r="Q33" s="62" t="inlineStr">
         <is>
           <t>已卖出清仓，没赚到</t>
         </is>
       </c>
-      <c r="R33" s="7" t="n"/>
-      <c r="S33" s="7" t="n"/>
+      <c r="R33" s="8" t="n"/>
+      <c r="S33" s="8" t="n"/>
       <c r="T33" s="0" t="n"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K2:K22">
+  <conditionalFormatting sqref="J2:J22">
     <cfRule priority="1" type="colorScale">
       <colorScale>
         <cfvo type="min"/>
@@ -3137,14 +3144,38 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K22">
+    <cfRule priority="4" type="colorScale">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K31:K33">
-    <cfRule dxfId="0" operator="lessThan" priority="5" type="cellIs">
+    <cfRule dxfId="0" operator="lessThan" priority="8" type="cellIs">
       <formula>-0.03</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:J22 A31:Q33 A23:Q23 L2:Q22">
-    <cfRule dxfId="1" operator="between" priority="4" text="卖出" type="containsText">
+  <conditionalFormatting sqref="A2:H22 A31:Q33 A23:Q23 L2:Q22">
+    <cfRule dxfId="1" operator="between" priority="7" text="卖出" type="containsText">
       <formula>NOT(ISERROR(SEARCH("卖出",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:J22">
+    <cfRule priority="3" type="colorScale">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -3168,14 +3199,14 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="9" width="14"/>
-    <col customWidth="1" max="4" min="4" style="9" width="35.5"/>
+    <col customWidth="1" max="1" min="1" style="1" width="14"/>
+    <col customWidth="1" max="4" min="4" style="1" width="35.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3201,13 +3232,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>43899</v>
       </c>
-      <c r="B2" s="64" t="n">
+      <c r="B2" s="63" t="n">
         <v>500</v>
       </c>
-      <c r="C2" s="3" t="inlineStr">
+      <c r="C2" s="4" t="inlineStr">
         <is>
           <t>005312</t>
         </is>
@@ -3218,56 +3249,56 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="3" s="9">
-      <c r="B3" s="64" t="n">
+    <row customHeight="1" ht="15.75" r="3" s="1">
+      <c r="B3" s="63" t="n">
         <v>500</v>
       </c>
-      <c r="C3" s="3" t="inlineStr">
+      <c r="C3" s="4" t="inlineStr">
         <is>
           <t>005963</t>
         </is>
       </c>
-      <c r="D3" s="4" t="inlineStr">
+      <c r="D3" s="5" t="inlineStr">
         <is>
           <t>宝盈人工智能股票C</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="64" t="n">
+      <c r="B4" s="63" t="n">
         <v>500</v>
       </c>
-      <c r="C4" s="3" t="inlineStr">
+      <c r="C4" s="4" t="inlineStr">
         <is>
           <t>000404</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
+      <c r="D4" s="6" t="inlineStr">
         <is>
           <t>易方达新兴成长灵活配置</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="64" t="n">
+      <c r="B5" s="63" t="n">
         <v>100</v>
       </c>
-      <c r="C5" s="6" t="inlineStr">
+      <c r="C5" s="7" t="inlineStr">
         <is>
           <t>161028</t>
         </is>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="8" t="inlineStr">
         <is>
           <t>富国中征信能源汽车指数分级</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="64" t="n">
+      <c r="B6" s="63" t="n">
         <v>500</v>
       </c>
-      <c r="C6" s="8" t="inlineStr">
+      <c r="C6" s="9" t="inlineStr">
         <is>
           <t>008087</t>
         </is>

</xml_diff>